<commit_message>
Refactor run_lsl.py to improve file naming conventions for recordings; update audio file naming to include run count. Update dropdown options in UI for block selection.
</commit_message>
<xml_diff>
--- a/results/sub-08/order_matrix_08_A_VR.xlsx
+++ b/results/sub-08/order_matrix_08_A_VR.xlsx
@@ -461,27 +461,27 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>dimension</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>order_emojis_slider</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>path</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>block_num</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>dimension</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>order_emojis_slider</t>
         </is>
       </c>
     </row>
@@ -503,19 +503,19 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>./instructions_videos/initial_relaxation_video_text.mp4</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
+          <t>./instructions_videos/initial_relaxation_video_text.mp4</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>initial_relaxation</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -535,19 +535,19 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>./calm_videos/VR/901.mp4</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
+          <t>./calm_videos/VR/901.mp4</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>calm_901</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -567,21 +567,21 @@
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>./instructions_videos/block_3_text.mp4</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
+          <t>./instructions_videos/block_1_text.mp4</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -604,30 +604,30 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/6.mp4</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>3</v>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>../stimuli/exp_videos/VR/8.mp4</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>valence</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>direct</t>
         </is>
       </c>
     </row>
@@ -649,21 +649,21 @@
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -683,21 +683,21 @@
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
         <is>
           <t>./videos_fixation/countdown_bar.mp4</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>verbal_report</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -717,21 +717,21 @@
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>3</v>
-      </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -751,21 +751,21 @@
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>./instructions_videos/block_3_text_reminder.mp4</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>3</v>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
+          <t>./instructions_videos/block_1_text_reminder.mp4</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -788,30 +788,30 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/13.mp4</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>3</v>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>../stimuli/exp_videos/VR/4.mp4</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>valence</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>direct</t>
         </is>
       </c>
     </row>
@@ -833,21 +833,21 @@
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
-      <c r="G11" t="n">
-        <v>3</v>
-      </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -867,21 +867,21 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
         <is>
           <t>./videos_fixation/countdown_bar.mp4</t>
         </is>
       </c>
-      <c r="G12" t="n">
-        <v>3</v>
-      </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>verbal_report</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -901,21 +901,21 @@
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G13" t="n">
-        <v>3</v>
-      </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -935,21 +935,21 @@
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>./instructions_videos/block_3_text_reminder.mp4</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>3</v>
-      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
+          <t>./instructions_videos/block_1_text_reminder.mp4</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -972,30 +972,30 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/14.mp4</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>3</v>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
+          <t>../stimuli/exp_videos/VR/7.mp4</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>valence</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>direct</t>
         </is>
       </c>
     </row>
@@ -1017,21 +1017,21 @@
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
-      <c r="G16" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="inlineStr">
         <is>
           <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1051,21 +1051,21 @@
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
         <is>
           <t>./videos_fixation/countdown_bar.mp4</t>
         </is>
       </c>
-      <c r="G17" t="n">
-        <v>3</v>
-      </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="inlineStr">
         <is>
           <t>verbal_report</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1085,21 +1085,21 @@
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G18" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1119,19 +1119,21 @@
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
-        </is>
-      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>luminance_instructions</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+          <t>./instructions_videos/block_1_text_reminder.mp4</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>audio_instruction</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1152,26 +1154,32 @@
       <c r="D20" t="n">
         <v>4</v>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/green_intensity_video_9.mp4</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr"/>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>luminance</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>luminance</t>
-        </is>
+          <t>../stimuli/exp_videos/VR/9.mp4</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>direct</t>
+          <t>video</t>
         </is>
       </c>
     </row>
@@ -1193,21 +1201,21 @@
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>./instructions_videos/block_1_text.mp4</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
         <v>1</v>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>audio_instruction</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>instruction_post_stimulus_verbal_report</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1225,35 +1233,21 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>5</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>../stimuli/exp_videos/VR/9.mp4</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>./videos_fixation/countdown_bar.mp4</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
         <v>1</v>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>video</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>direct</t>
+          <t>verbal_report</t>
         </is>
       </c>
     </row>
@@ -1275,21 +1269,21 @@
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>./black_screen_5_sec.mp4</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
         <v>1</v>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>instruction_post_stimulus_verbal_report</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>black_screen_5_seconds</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1309,21 +1303,19 @@
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>./videos_fixation/countdown_bar.mp4</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
-        <v>1</v>
-      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>verbal_report</t>
+          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>luminance_instructions</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1341,23 +1333,31 @@
           <t>VR</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>5</v>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>./black_screen_5_sec.mp4</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>1</v>
+          <t>luminance</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>black_screen_5_seconds</t>
+          <t>../stimuli/exp_videos/VR/green_intensity_video_3.mp4</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>luminance</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1377,21 +1377,21 @@
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>./instructions_videos/block_1_text_reminder.mp4</t>
-        </is>
-      </c>
-      <c r="G26" t="n">
-        <v>1</v>
-      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
+          <t>./instructions_videos/block_3_text.mp4</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>3</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1414,30 +1414,30 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/8.mp4</t>
-        </is>
-      </c>
-      <c r="G27" t="n">
-        <v>1</v>
+          <t>valence</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
+          <t>../stimuli/exp_videos/VR/13.mp4</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>direct</t>
         </is>
       </c>
     </row>
@@ -1459,21 +1459,21 @@
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
-      <c r="G28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="n">
+        <v>3</v>
+      </c>
+      <c r="J28" t="inlineStr">
         <is>
           <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1493,21 +1493,21 @@
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
         <is>
           <t>./videos_fixation/countdown_bar.mp4</t>
         </is>
       </c>
-      <c r="G29" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="n">
+        <v>3</v>
+      </c>
+      <c r="J29" t="inlineStr">
         <is>
           <t>verbal_report</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1527,21 +1527,21 @@
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr">
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G30" t="n">
-        <v>1</v>
-      </c>
-      <c r="H30" t="inlineStr">
+      <c r="I30" t="n">
+        <v>3</v>
+      </c>
+      <c r="J30" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1561,21 +1561,21 @@
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>./instructions_videos/block_1_text_reminder.mp4</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
-        <v>1</v>
-      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
+          <t>./instructions_videos/block_3_text_reminder.mp4</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>3</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1598,30 +1598,30 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/4.mp4</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
-        <v>1</v>
+          <t>valence</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
+          <t>../stimuli/exp_videos/VR/6.mp4</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>direct</t>
         </is>
       </c>
     </row>
@@ -1643,21 +1643,21 @@
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr">
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
-      <c r="G33" t="n">
-        <v>1</v>
-      </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="n">
+        <v>3</v>
+      </c>
+      <c r="J33" t="inlineStr">
         <is>
           <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1677,21 +1677,21 @@
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr">
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
         <is>
           <t>./videos_fixation/countdown_bar.mp4</t>
         </is>
       </c>
-      <c r="G34" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="n">
+        <v>3</v>
+      </c>
+      <c r="J34" t="inlineStr">
         <is>
           <t>verbal_report</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1711,21 +1711,21 @@
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G35" t="n">
-        <v>1</v>
-      </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="n">
+        <v>3</v>
+      </c>
+      <c r="J35" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1745,21 +1745,21 @@
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>./instructions_videos/block_1_text_reminder.mp4</t>
-        </is>
-      </c>
-      <c r="G36" t="n">
-        <v>1</v>
-      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
+          <t>./instructions_videos/block_3_text_reminder.mp4</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>3</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1782,30 +1782,30 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/7.mp4</t>
-        </is>
-      </c>
-      <c r="G37" t="n">
-        <v>1</v>
+          <t>valence</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
+          <t>../stimuli/exp_videos/VR/14.mp4</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>3</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>direct</t>
         </is>
       </c>
     </row>
@@ -1827,21 +1827,21 @@
       </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr">
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
-      <c r="G38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="n">
+        <v>3</v>
+      </c>
+      <c r="J38" t="inlineStr">
         <is>
           <t>instruction_post_stimulus_verbal_report</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1861,21 +1861,21 @@
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
         <is>
           <t>./videos_fixation/countdown_bar.mp4</t>
         </is>
       </c>
-      <c r="G39" t="n">
-        <v>1</v>
-      </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="n">
+        <v>3</v>
+      </c>
+      <c r="J39" t="inlineStr">
         <is>
           <t>verbal_report</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1895,21 +1895,21 @@
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G40" t="n">
-        <v>1</v>
-      </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="n">
+        <v>3</v>
+      </c>
+      <c r="J40" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1929,19 +1929,19 @@
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
-        </is>
-      </c>
+      <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
+          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
           <t>luminance_instructions</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1965,23 +1965,23 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/green_intensity_video_3.mp4</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
+          <t>luminance</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>direct</t>
+        </is>
+      </c>
       <c r="H42" t="inlineStr">
         <is>
+          <t>../stimuli/exp_videos/VR/green_intensity_video_9.mp4</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr">
+        <is>
           <t>luminance</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>luminance</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>direct</t>
         </is>
       </c>
     </row>
@@ -2003,21 +2003,21 @@
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
         <is>
           <t>./instructions_videos/block_2_text.mp4</t>
         </is>
       </c>
-      <c r="G43" t="n">
+      <c r="I43" t="n">
         <v>2</v>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="J43" t="inlineStr">
         <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2040,30 +2040,30 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/10.mp4</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">inverse </t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>../stimuli/exp_videos/VR/1.mp4</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
         <v>2</v>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="J44" t="inlineStr">
         <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>inverse</t>
         </is>
       </c>
     </row>
@@ -2085,21 +2085,21 @@
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr">
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
-      <c r="G45" t="n">
+      <c r="I45" t="n">
         <v>2</v>
       </c>
-      <c r="H45" t="inlineStr">
+      <c r="J45" t="inlineStr">
         <is>
           <t>post_stimulus_self_report</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2119,21 +2119,21 @@
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G46" t="n">
+      <c r="I46" t="n">
         <v>2</v>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="J46" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2153,21 +2153,21 @@
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
         <is>
           <t>./instructions_videos/block_2_text_reminder.mp4</t>
         </is>
       </c>
-      <c r="G47" t="n">
+      <c r="I47" t="n">
         <v>2</v>
       </c>
-      <c r="H47" t="inlineStr">
+      <c r="J47" t="inlineStr">
         <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2190,30 +2190,30 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/1.mp4</t>
-        </is>
-      </c>
-      <c r="G48" t="n">
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>../stimuli/exp_videos/VR/10.mp4</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
         <v>2</v>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="J48" t="inlineStr">
         <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t xml:space="preserve">inverse </t>
         </is>
       </c>
     </row>
@@ -2235,21 +2235,21 @@
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr">
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
-      <c r="G49" t="n">
+      <c r="I49" t="n">
         <v>2</v>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="J49" t="inlineStr">
         <is>
           <t>post_stimulus_self_report</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2269,21 +2269,21 @@
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr">
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G50" t="n">
+      <c r="I50" t="n">
         <v>2</v>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="J50" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2303,21 +2303,21 @@
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr">
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
         <is>
           <t>./instructions_videos/block_2_text_reminder.mp4</t>
         </is>
       </c>
-      <c r="G51" t="n">
+      <c r="I51" t="n">
         <v>2</v>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="J51" t="inlineStr">
         <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2345,25 +2345,25 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
           <t>../stimuli/exp_videos/VR/11.mp4</t>
         </is>
       </c>
-      <c r="G52" t="n">
+      <c r="I52" t="n">
         <v>2</v>
       </c>
-      <c r="H52" t="inlineStr">
+      <c r="J52" t="inlineStr">
         <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>inverse</t>
         </is>
       </c>
     </row>
@@ -2385,21 +2385,21 @@
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr">
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
-      <c r="G53" t="n">
+      <c r="I53" t="n">
         <v>2</v>
       </c>
-      <c r="H53" t="inlineStr">
+      <c r="J53" t="inlineStr">
         <is>
           <t>post_stimulus_self_report</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2419,21 +2419,21 @@
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr">
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G54" t="n">
+      <c r="I54" t="n">
         <v>2</v>
       </c>
-      <c r="H54" t="inlineStr">
+      <c r="J54" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2453,21 +2453,21 @@
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr">
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr">
         <is>
           <t>./instructions_videos/block_2_text_reminder.mp4</t>
         </is>
       </c>
-      <c r="G55" t="n">
+      <c r="I55" t="n">
         <v>2</v>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="J55" t="inlineStr">
         <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2495,25 +2495,25 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
+          <t>arousal</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
           <t>../stimuli/exp_videos/VR/5.mp4</t>
         </is>
       </c>
-      <c r="G56" t="n">
+      <c r="I56" t="n">
         <v>2</v>
       </c>
-      <c r="H56" t="inlineStr">
+      <c r="J56" t="inlineStr">
         <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>arousal</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>inverse</t>
         </is>
       </c>
     </row>
@@ -2535,21 +2535,21 @@
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr">
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
-      <c r="G57" t="n">
+      <c r="I57" t="n">
         <v>2</v>
       </c>
-      <c r="H57" t="inlineStr">
+      <c r="J57" t="inlineStr">
         <is>
           <t>post_stimulus_self_report</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2569,21 +2569,21 @@
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr">
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G58" t="n">
+      <c r="I58" t="n">
         <v>2</v>
       </c>
-      <c r="H58" t="inlineStr">
+      <c r="J58" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I58" t="inlineStr"/>
-      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2603,19 +2603,19 @@
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>./instructions_videos/luminance_instructions_inverse.mp4</t>
-        </is>
-      </c>
+      <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
+          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr">
+        <is>
           <t>luminance_instructions</t>
         </is>
       </c>
-      <c r="I59" t="inlineStr"/>
-      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2639,23 +2639,23 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
+          <t>luminance</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">inverse </t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
           <t>../stimuli/exp_videos/VR/green_intensity_video_7.mp4</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr">
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr">
         <is>
           <t>luminance</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>luminance</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>inverse</t>
         </is>
       </c>
     </row>
@@ -2677,21 +2677,21 @@
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr">
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr">
         <is>
           <t>./instructions_videos/block_4_text.mp4</t>
         </is>
       </c>
-      <c r="G61" t="n">
+      <c r="I61" t="n">
         <v>4</v>
       </c>
-      <c r="H61" t="inlineStr">
+      <c r="J61" t="inlineStr">
         <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2719,25 +2719,25 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
+          <t>valence</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
           <t>../stimuli/exp_videos/VR/3.mp4</t>
         </is>
       </c>
-      <c r="G62" t="n">
+      <c r="I62" t="n">
         <v>4</v>
       </c>
-      <c r="H62" t="inlineStr">
+      <c r="J62" t="inlineStr">
         <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>valence</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>inverse</t>
         </is>
       </c>
     </row>
@@ -2759,21 +2759,21 @@
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr">
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
-      <c r="G63" t="n">
+      <c r="I63" t="n">
         <v>4</v>
       </c>
-      <c r="H63" t="inlineStr">
+      <c r="J63" t="inlineStr">
         <is>
           <t>post_stimulus_self_report</t>
         </is>
       </c>
-      <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2793,21 +2793,21 @@
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr">
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G64" t="n">
+      <c r="I64" t="n">
         <v>4</v>
       </c>
-      <c r="H64" t="inlineStr">
+      <c r="J64" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I64" t="inlineStr"/>
-      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2827,21 +2827,21 @@
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
-      <c r="F65" t="inlineStr">
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr">
         <is>
           <t>./instructions_videos/block_4_text_reminder.mp4</t>
         </is>
       </c>
-      <c r="G65" t="n">
+      <c r="I65" t="n">
         <v>4</v>
       </c>
-      <c r="H65" t="inlineStr">
+      <c r="J65" t="inlineStr">
         <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr"/>
-      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2864,30 +2864,30 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/12.mp4</t>
-        </is>
-      </c>
-      <c r="G66" t="n">
+          <t>valence</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>../stimuli/exp_videos/VR/2.mp4</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
         <v>4</v>
       </c>
-      <c r="H66" t="inlineStr">
+      <c r="J66" t="inlineStr">
         <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>valence</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>inverse</t>
         </is>
       </c>
     </row>
@@ -2909,21 +2909,21 @@
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr">
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
-      <c r="G67" t="n">
+      <c r="I67" t="n">
         <v>4</v>
       </c>
-      <c r="H67" t="inlineStr">
+      <c r="J67" t="inlineStr">
         <is>
           <t>post_stimulus_self_report</t>
         </is>
       </c>
-      <c r="I67" t="inlineStr"/>
-      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2943,21 +2943,21 @@
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
-      <c r="F68" t="inlineStr">
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G68" t="n">
+      <c r="I68" t="n">
         <v>4</v>
       </c>
-      <c r="H68" t="inlineStr">
+      <c r="J68" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2977,21 +2977,21 @@
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr">
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
         <is>
           <t>./instructions_videos/block_4_text_reminder.mp4</t>
         </is>
       </c>
-      <c r="G69" t="n">
+      <c r="I69" t="n">
         <v>4</v>
       </c>
-      <c r="H69" t="inlineStr">
+      <c r="J69" t="inlineStr">
         <is>
           <t>audio_instruction</t>
         </is>
       </c>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3014,30 +3014,30 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/2.mp4</t>
-        </is>
-      </c>
-      <c r="G70" t="n">
+          <t>valence</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>../stimuli/exp_videos/VR/12.mp4</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
         <v>4</v>
       </c>
-      <c r="H70" t="inlineStr">
+      <c r="J70" t="inlineStr">
         <is>
           <t>video</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>valence</t>
-        </is>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>inverse</t>
         </is>
       </c>
     </row>
@@ -3059,21 +3059,21 @@
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr">
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
         <is>
           <t>./instructions_videos/post_stimulus_self_report.mp4</t>
         </is>
       </c>
-      <c r="G71" t="n">
+      <c r="I71" t="n">
         <v>4</v>
       </c>
-      <c r="H71" t="inlineStr">
+      <c r="J71" t="inlineStr">
         <is>
           <t>post_stimulus_self_report</t>
         </is>
       </c>
-      <c r="I71" t="inlineStr"/>
-      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3093,21 +3093,21 @@
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr">
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr">
         <is>
           <t>./black_screen_5_sec.mp4</t>
         </is>
       </c>
-      <c r="G72" t="n">
+      <c r="I72" t="n">
         <v>4</v>
       </c>
-      <c r="H72" t="inlineStr">
+      <c r="J72" t="inlineStr">
         <is>
           <t>black_screen_5_seconds</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr"/>
-      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3127,19 +3127,19 @@
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>./instructions_videos/luminance_instructions_inverse.mp4</t>
-        </is>
-      </c>
+      <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr">
         <is>
+          <t>./instructions_videos/luminance_instructions_inverse.mp4</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr">
+        <is>
           <t>luminance_instructions</t>
         </is>
       </c>
-      <c r="I73" t="inlineStr"/>
-      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3163,23 +3163,23 @@
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
+          <t>luminance</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>inverse</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
           <t>../stimuli/exp_videos/VR/green_intensity_video_12.mp4</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr">
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr">
         <is>
           <t>luminance</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>luminance</t>
-        </is>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>inverse</t>
         </is>
       </c>
     </row>
@@ -3201,19 +3201,19 @@
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>./instructions_videos/rest_suprablock_text.mp4</t>
-        </is>
-      </c>
+      <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr">
         <is>
+          <t>./instructions_videos/rest_suprablock_text.mp4</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr">
+        <is>
           <t>rest_suprablock</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr"/>
-      <c r="J75" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>